<commit_message>
Added Pekka experimental project folder from git & updated many conversion scripts
</commit_message>
<xml_diff>
--- a/Documentation/Scope.xlsx
+++ b/Documentation/Scope.xlsx
@@ -2,10 +2,10 @@
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <fileVersion appName="Calc"/>
-  <workbookPr backupFile="false" showObjects="all" dateCompatibility="false"/>
+  <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="3"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Phase 1 (current)" sheetId="1" state="visible" r:id="rId3"/>
@@ -64,6 +64,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">Styling, links etc. to wait until a 2</t>
     </r>
@@ -73,6 +74,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">nd</t>
     </r>
@@ -81,6 +83,7 @@
         <sz val="10"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve"> pass</t>
     </r>
@@ -128,61 +131,13 @@
     <t xml:space="preserve">Sample run environments</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">See </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">RF libs &gt; xml</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> for an example</t>
-    </r>
+    <t xml:space="preserve">See RF libs &gt; xml for an example</t>
   </si>
   <si>
     <t xml:space="preserve">Sample gif with typing</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">See </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">this stackoverflow page</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> for an example</t>
-    </r>
+    <t xml:space="preserve">See this stackoverflow page for an example</t>
   </si>
   <si>
     <t xml:space="preserve">Light &amp; dark mode</t>
@@ -194,31 +149,7 @@
     <t xml:space="preserve">Coloured block notes &amp; tips</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">See </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <color rgb="FF0000FF"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">this example</t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve"> to make them separated &amp; clearer</t>
-    </r>
+    <t xml:space="preserve">See this example to make them separated &amp; clearer</t>
   </si>
   <si>
     <t xml:space="preserve">Compare RF to other tools</t>
@@ -227,7 +158,7 @@
     <t xml:space="preserve">RF vs specflow/cucumber page etc.</t>
   </si>
   <si>
-    <t xml:space="preserve">[WON’T DO]</t>
+    <t xml:space="preserve">Some other tools have this. Useful???</t>
   </si>
   <si>
     <t xml:space="preserve">Source code</t>
@@ -284,6 +215,7 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -312,12 +244,14 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
       <color rgb="FF0000FF"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
   </fonts>
   <fills count="3">
@@ -375,8 +309,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -384,7 +322,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="true">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -397,23 +339,6 @@
     <cellStyle name="Currency [0]" xfId="18" builtinId="7"/>
     <cellStyle name="Percent" xfId="19" builtinId="5"/>
   </cellStyles>
-  <dxfs count="2">
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <fgColor rgb="FFFFE994"/>
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill patternType="solid">
-          <bgColor rgb="FF000000"/>
-        </patternFill>
-      </fill>
-    </dxf>
-  </dxfs>
   <colors>
     <indexedColors>
       <rgbColor rgb="FF000000"/>
@@ -591,81 +516,81 @@
   <dimension ref="A1:D5"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C9" activeCellId="0" sqref="C9"/>
+      <selection pane="topLeft" activeCell="D2" activeCellId="0" sqref="D2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="38.95"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="57.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="38.94"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="57.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D2" s="0" t="s">
+      <c r="D2" s="1" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D3" s="0" t="s">
+      <c r="D3" s="1" t="s">
         <v>10</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>6</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="C5" s="0" t="s">
+      <c r="C5" s="1" t="s">
         <v>6</v>
       </c>
     </row>
@@ -694,108 +619,108 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C6" activeCellId="0" sqref="C6"/>
+      <selection pane="topLeft" activeCell="C2" activeCellId="0" sqref="C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="44.04"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="57.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="44.04"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="57.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="C2" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="0" t="s">
+      <c r="B3" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="C3" s="2" t="s">
+      <c r="C3" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="B4" s="0" t="s">
+      <c r="B4" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="C4" s="2" t="s">
+      <c r="C4" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="D4" s="0" t="s">
+      <c r="D4" s="1" t="s">
         <v>23</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="B5" s="0" t="s">
+      <c r="B5" s="4" t="s">
         <v>25</v>
       </c>
-      <c r="C5" s="2" t="s">
+      <c r="C5" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>26</v>
       </c>
-      <c r="B6" s="0" t="s">
+      <c r="B6" s="4" t="s">
         <v>27</v>
       </c>
-      <c r="C6" s="2" t="s">
+      <c r="C6" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>28</v>
       </c>
-      <c r="B7" s="0" t="s">
+      <c r="B7" s="1" t="s">
         <v>29</v>
       </c>
-      <c r="C7" s="2" t="s">
+      <c r="C7" s="3" t="s">
         <v>18</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="13" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>30</v>
       </c>
-      <c r="B8" s="0" t="s">
+      <c r="B8" s="4" t="s">
         <v>31</v>
       </c>
-      <c r="C8" s="2" t="s">
+      <c r="C8" s="3" t="s">
         <v>18</v>
       </c>
     </row>
@@ -807,9 +732,9 @@
     </dataValidation>
   </dataValidations>
   <hyperlinks>
-    <hyperlink ref="B5" r:id="rId1" location="xml-library" display="RF libs &gt; xml"/>
-    <hyperlink ref="B6" r:id="rId2" display="this stackoverflow page"/>
-    <hyperlink ref="B8" r:id="rId3" display="this example"/>
+    <hyperlink ref="B5" r:id="rId1" location="xml-library" display="See RF libs &gt; xml for an example"/>
+    <hyperlink ref="B6" r:id="rId2" display="See this stackoverflow page for an example"/>
+    <hyperlink ref="B8" r:id="rId3" display="See this example to make them separated &amp; clearer"/>
   </hyperlinks>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
@@ -828,51 +753,51 @@
   </sheetPr>
   <dimension ref="A1:D4"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="C5" activeCellId="0" sqref="C5"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="A1" activeCellId="0" sqref="A1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="25.93"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="36.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="57.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="25.93"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="36.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="57.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>32</v>
       </c>
-      <c r="B2" s="0" t="s">
+      <c r="B2" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="C2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D2" s="0" t="s">
+      <c r="C2" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D2" s="1" t="s">
         <v>34</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C3" s="2"/>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="C4" s="2"/>
+      <c r="C4" s="3"/>
     </row>
   </sheetData>
   <dataValidations count="1">
@@ -898,106 +823,106 @@
   </sheetPr>
   <dimension ref="A1:D16"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="A18" activeCellId="0" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="0" width="36.03"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="15.28"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="0" width="57.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="1" style="1" width="36.03"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="57.41"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1" t="s">
+      <c r="B1" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="1" t="s">
+      <c r="C1" s="2" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>35</v>
       </c>
-      <c r="C2" s="2"/>
+      <c r="C2" s="3"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="2"/>
+      <c r="C3" s="3"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="s">
+      <c r="A4" s="1" t="s">
         <v>37</v>
       </c>
-      <c r="C4" s="2"/>
+      <c r="C4" s="3"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="s">
+      <c r="A5" s="1" t="s">
         <v>38</v>
       </c>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A6" s="0" t="s">
+      <c r="A6" s="1" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A7" s="0" t="s">
+      <c r="A7" s="1" t="s">
         <v>40</v>
       </c>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A8" s="0" t="s">
+      <c r="A8" s="1" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="s">
+      <c r="A9" s="1" t="s">
         <v>42</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="s">
+      <c r="A10" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="s">
+      <c r="A11" s="1" t="s">
         <v>44</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="s">
+      <c r="A12" s="1" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="s">
+      <c r="A13" s="1" t="s">
         <v>46</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="s">
+      <c r="A14" s="1" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="s">
+      <c r="A15" s="1" t="s">
         <v>47</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="s">
+      <c r="A16" s="1" t="s">
         <v>48</v>
       </c>
     </row>
@@ -1032,21 +957,21 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="15.28"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="15.28"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A2" s="0" t="s">
+      <c r="A2" s="1" t="s">
         <v>6</v>
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="s">
+      <c r="A3" s="1" t="s">
         <v>18</v>
       </c>
     </row>

</xml_diff>